<commit_message>
fifth commit- albums working, change to mp3
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24860" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="SongList" sheetId="2" r:id="rId2"/>
+    <sheet name="Status" sheetId="3" r:id="rId2"/>
+    <sheet name="SongList" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="194">
   <si>
     <t>Album Match</t>
   </si>
@@ -364,9 +365,6 @@
     <t>https://www.youtube.com/watch?v=E1fzJ_AYajA</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Death From Above 1979</t>
   </si>
   <si>
@@ -554,6 +552,57 @@
   </si>
   <si>
     <t>displays both scores</t>
+  </si>
+  <si>
+    <t>Queens of the Stone Age</t>
+  </si>
+  <si>
+    <t>Them Crooked Vultures</t>
+  </si>
+  <si>
+    <t>Jay Z</t>
+  </si>
+  <si>
+    <t>Beyonce</t>
+  </si>
+  <si>
+    <t>Taylor Swift</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>function songPlay</t>
+  </si>
+  <si>
+    <t>function logPoint</t>
+  </si>
+  <si>
+    <t>function displayCorrectWrong</t>
+  </si>
+  <si>
+    <t>will log a point if the correct album is clicked</t>
+  </si>
+  <si>
+    <t>displays a document.write depending if answer is correct or not</t>
+  </si>
+  <si>
+    <t>function displayScores</t>
+  </si>
+  <si>
+    <t>needs to play one of the 4 songs by populating the audio tag in the html page</t>
+  </si>
+  <si>
+    <t>needs to randomly choose the song from the album array</t>
+  </si>
+  <si>
+    <t>make this a function of the getWinner function</t>
+  </si>
+  <si>
+    <t>ITEMS TO COMPLETE</t>
+  </si>
+  <si>
+    <t>how to pull a Var into a document.write function</t>
   </si>
 </sst>
 </file>
@@ -767,7 +816,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -861,8 +910,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -885,13 +960,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -909,8 +981,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -957,6 +1035,19 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1003,6 +1094,19 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1332,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I100"/>
+  <dimension ref="A2:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1347,14 +1451,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="30">
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" s="1" t="s">
@@ -1460,10 +1564,10 @@
     <row r="13" spans="2:9">
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
     </row>
@@ -1510,10 +1614,10 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="3"/>
       <c r="I20" s="4"/>
     </row>
@@ -1539,10 +1643,10 @@
     <row r="23" spans="2:9">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="20"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="3"/>
       <c r="I23" s="4"/>
     </row>
@@ -1627,17 +1731,21 @@
     <row r="32" spans="2:9">
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="21"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="10"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="1:9">
       <c r="B34" s="1"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="1:9">
+      <c r="A36" s="20"/>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
@@ -1645,17 +1753,25 @@
       <c r="H36" s="13"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="1:9">
+      <c r="A37" s="20"/>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="20"/>
+      <c r="G37" s="21"/>
       <c r="H37" s="3"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="1:9">
+      <c r="A38" s="20"/>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1663,7 +1779,11 @@
       <c r="H38" s="3"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="1:9">
+      <c r="A39" s="20"/>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1671,17 +1791,25 @@
       <c r="H39" s="3"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="1:9">
+      <c r="A40" s="20"/>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
       <c r="D40" s="2"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="20"/>
+      <c r="G40" s="21"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="1:9">
+      <c r="A41" s="20"/>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
       <c r="D41" s="2"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1689,7 +1817,8 @@
       <c r="H41" s="3"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="1:9">
+      <c r="A42" s="20"/>
       <c r="D42" s="2"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1697,7 +1826,11 @@
       <c r="H42" s="3"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="1:9">
+      <c r="A43" s="20"/>
+      <c r="B43" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
@@ -1705,9 +1838,10 @@
       <c r="H43" s="15"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="1" t="s">
-        <v>92</v>
+    <row r="44" spans="1:9">
+      <c r="A44" s="20"/>
+      <c r="B44" t="s">
+        <v>97</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="16"/>
@@ -1716,9 +1850,10 @@
       <c r="H44" s="16"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="1:9">
+      <c r="A45" s="20"/>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="16"/>
@@ -1727,9 +1862,10 @@
       <c r="H45" s="16"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="1:9">
+      <c r="A46" s="20"/>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="17"/>
@@ -1738,9 +1874,10 @@
       <c r="H46" s="17"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="1:9">
+      <c r="A47" s="20"/>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="18" t="s">
@@ -1757,9 +1894,10 @@
       </c>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="2:9">
+    <row r="48" spans="1:9">
+      <c r="A48" s="20"/>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="3"/>
@@ -1768,32 +1906,37 @@
       <c r="H48" s="3"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="2:9">
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
+    <row r="49" spans="1:9">
+      <c r="A49" s="20"/>
+      <c r="B49" s="1"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
-      <c r="F49" s="21" t="s">
+      <c r="F49" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G49" s="21"/>
+      <c r="G49" s="27"/>
       <c r="H49" s="10"/>
       <c r="I49" s="11"/>
     </row>
-    <row r="51" spans="2:9">
-      <c r="B51" s="1" t="s">
+    <row r="50" spans="1:9">
+      <c r="A50" s="20"/>
+      <c r="B50" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="20"/>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="20"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="20"/>
+      <c r="B53" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9">
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9">
-      <c r="B53" t="s">
-        <v>98</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="13"/>
@@ -1802,22 +1945,24 @@
       <c r="H53" s="13"/>
       <c r="I53" s="14"/>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="1:9">
+      <c r="A54" s="20"/>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="20"/>
+      <c r="G54" s="21"/>
       <c r="H54" s="3"/>
       <c r="I54" s="4"/>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="1:9">
+      <c r="A55" s="20"/>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="3"/>
@@ -1826,9 +1971,10 @@
       <c r="H55" s="3"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="1:9">
+      <c r="A56" s="20"/>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="3"/>
@@ -1837,8 +1983,11 @@
       <c r="H56" s="3"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="2:9">
-      <c r="B57" s="1"/>
+    <row r="57" spans="1:9">
+      <c r="A57" s="20"/>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
       <c r="D57" s="2"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -1846,23 +1995,22 @@
       <c r="H57" s="3"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="2:9">
-      <c r="B58" s="1" t="s">
-        <v>101</v>
+    <row r="58" spans="1:9">
+      <c r="A58" s="20"/>
+      <c r="B58" t="s">
+        <v>100</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="20" t="s">
+      <c r="F58" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G58" s="20"/>
+      <c r="G58" s="21"/>
       <c r="H58" s="3"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" spans="2:9">
-      <c r="B59" t="s">
-        <v>104</v>
-      </c>
+    <row r="59" spans="1:9">
+      <c r="A59" s="20"/>
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -1870,19 +2018,26 @@
       <c r="H59" s="3"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="1:9">
+      <c r="A60" s="20"/>
+      <c r="B60" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D60" s="2"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G60" s="20"/>
+      <c r="G60" s="21"/>
       <c r="H60" s="3"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="2:9">
-      <c r="B61" s="1" t="s">
-        <v>96</v>
+    <row r="61" spans="1:9">
+      <c r="A61" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="3"/>
@@ -1891,9 +2046,10 @@
       <c r="H61" s="3"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="1:9">
+      <c r="A62" s="20"/>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="3"/>
@@ -1902,9 +2058,10 @@
       <c r="H62" s="3"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="1:9">
+      <c r="A63" s="20"/>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
@@ -1913,10 +2070,7 @@
       <c r="H63" s="3"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="2:9">
-      <c r="B64" t="s">
-        <v>99</v>
-      </c>
+    <row r="64" spans="1:9">
       <c r="D64" s="2"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
@@ -1924,10 +2078,7 @@
       <c r="H64" s="18"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="2:9">
-      <c r="B65" t="s">
-        <v>103</v>
-      </c>
+    <row r="65" spans="4:9">
       <c r="D65" s="2"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -1935,10 +2086,7 @@
       <c r="H65" s="3"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="2:9">
-      <c r="B66" t="s">
-        <v>100</v>
-      </c>
+    <row r="66" spans="4:9">
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
       <c r="F66" s="19"/>
@@ -1946,20 +2094,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="11"/>
     </row>
-    <row r="68" spans="2:9">
-      <c r="B68" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9">
-      <c r="B69" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9">
-      <c r="B70" t="s">
-        <v>177</v>
-      </c>
+    <row r="70" spans="4:9">
       <c r="D70" s="12"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -1967,20 +2102,17 @@
       <c r="H70" s="13"/>
       <c r="I70" s="14"/>
     </row>
-    <row r="71" spans="2:9">
-      <c r="B71" t="s">
-        <v>106</v>
-      </c>
+    <row r="71" spans="4:9">
       <c r="D71" s="2"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="20" t="s">
+      <c r="F71" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G71" s="20"/>
+      <c r="G71" s="21"/>
       <c r="H71" s="3"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="2:9">
+    <row r="72" spans="4:9">
       <c r="D72" s="2"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -1988,7 +2120,7 @@
       <c r="H72" s="3"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="2:9">
+    <row r="73" spans="4:9">
       <c r="D73" s="2"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -1996,17 +2128,17 @@
       <c r="H73" s="3"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="2:9">
+    <row r="74" spans="4:9">
       <c r="D74" s="2"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="20" t="s">
+      <c r="F74" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G74" s="20"/>
+      <c r="G74" s="21"/>
       <c r="H74" s="3"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="2:9">
+    <row r="75" spans="4:9">
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -2014,7 +2146,7 @@
       <c r="H75" s="3"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="2:9">
+    <row r="76" spans="4:9">
       <c r="D76" s="2"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -2022,7 +2154,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="2:9">
+    <row r="77" spans="4:9">
       <c r="D77" s="2"/>
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
@@ -2030,7 +2162,7 @@
       <c r="H77" s="15"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="2:9">
+    <row r="78" spans="4:9">
       <c r="D78" s="2"/>
       <c r="E78" s="16"/>
       <c r="F78" s="16"/>
@@ -2038,7 +2170,7 @@
       <c r="H78" s="16"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="2:9">
+    <row r="79" spans="4:9">
       <c r="D79" s="2"/>
       <c r="E79" s="16"/>
       <c r="F79" s="16"/>
@@ -2046,7 +2178,7 @@
       <c r="H79" s="16"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="2:9">
+    <row r="80" spans="4:9">
       <c r="D80" s="2"/>
       <c r="E80" s="17"/>
       <c r="F80" s="17"/>
@@ -2081,10 +2213,10 @@
     <row r="83" spans="4:9">
       <c r="D83" s="9"/>
       <c r="E83" s="10"/>
-      <c r="F83" s="21" t="s">
+      <c r="F83" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G83" s="21"/>
+      <c r="G83" s="27"/>
       <c r="H83" s="10"/>
       <c r="I83" s="11"/>
     </row>
@@ -2099,10 +2231,10 @@
     <row r="88" spans="4:9" ht="25">
       <c r="D88" s="2"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="22" t="s">
+      <c r="F88" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G88" s="22"/>
+      <c r="G88" s="28"/>
       <c r="H88" s="3"/>
       <c r="I88" s="4"/>
     </row>
@@ -2136,14 +2268,14 @@
     </row>
     <row r="93" spans="4:9">
       <c r="D93" s="2"/>
-      <c r="E93" s="20" t="s">
+      <c r="E93" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20" t="s">
+      <c r="F93" s="21"/>
+      <c r="G93" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H93" s="20"/>
+      <c r="H93" s="21"/>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="4:9">
@@ -2156,14 +2288,14 @@
     </row>
     <row r="95" spans="4:9">
       <c r="D95" s="2"/>
-      <c r="E95" s="20" t="s">
+      <c r="E95" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20" t="s">
+      <c r="F95" s="21"/>
+      <c r="G95" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H95" s="20"/>
+      <c r="H95" s="21"/>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="4:9">
@@ -2176,14 +2308,14 @@
     </row>
     <row r="97" spans="4:9">
       <c r="D97" s="2"/>
-      <c r="E97" s="20" t="s">
+      <c r="E97" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F97" s="20"/>
-      <c r="G97" s="20" t="s">
+      <c r="F97" s="21"/>
+      <c r="G97" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H97" s="20"/>
+      <c r="H97" s="21"/>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="4:9">
@@ -2212,6 +2344,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="G95:H95"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="F13:G13"/>
@@ -2224,15 +2365,6 @@
     <mergeCell ref="F54:G54"/>
     <mergeCell ref="F58:G58"/>
     <mergeCell ref="F60:G60"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="G95:H95"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2246,595 +2378,601 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="B2:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="147.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="147.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>119</v>
       </c>
       <c r="C6" t="s">
         <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B7" t="s">
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>6</v>
+      <c r="B8" t="s">
+        <v>122</v>
       </c>
       <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
         <v>123</v>
       </c>
-      <c r="D8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>7</v>
+      <c r="B9" t="s">
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>8</v>
+      <c r="B10" t="s">
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>9</v>
+      <c r="B11" t="s">
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12">
-        <v>10</v>
+      <c r="B12" t="s">
+        <v>156</v>
       </c>
       <c r="C12" t="s">
         <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>11</v>
+      <c r="B13" t="s">
+        <v>154</v>
       </c>
       <c r="C13" t="s">
         <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>12</v>
+      <c r="B14" t="s">
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>13</v>
+      <c r="B15" t="s">
+        <v>164</v>
       </c>
       <c r="C15" t="s">
         <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>14</v>
+      <c r="B16" t="s">
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>15</v>
+      <c r="B17" t="s">
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>16</v>
+      <c r="B18" t="s">
+        <v>147</v>
       </c>
       <c r="C18" t="s">
         <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19">
-        <v>17</v>
+      <c r="B19" t="s">
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>18</v>
+      <c r="B20" t="s">
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>19</v>
+      <c r="B21" t="s">
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>131</v>
       </c>
       <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
         <v>132</v>
-      </c>
-      <c r="E21" t="s">
-        <v>115</v>
       </c>
       <c r="F21" t="s">
         <v>133</v>
       </c>
-      <c r="G21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22">
-        <v>20</v>
+      <c r="B22" t="s">
+        <v>142</v>
       </c>
       <c r="C22" t="s">
         <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="F22" t="s">
         <v>135</v>
       </c>
-      <c r="G22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23">
-        <v>21</v>
+      <c r="B23" t="s">
+        <v>138</v>
       </c>
       <c r="C23" t="s">
         <v>139</v>
       </c>
       <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
         <v>140</v>
-      </c>
-      <c r="E23" t="s">
-        <v>117</v>
       </c>
       <c r="F23" t="s">
         <v>141</v>
       </c>
-      <c r="G23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24">
-        <v>22</v>
+      <c r="B24" t="s">
+        <v>149</v>
       </c>
       <c r="C24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s">
         <v>150</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" t="s">
         <v>152</v>
       </c>
-      <c r="E24" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25">
-        <v>23</v>
+      <c r="B25" t="s">
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>161</v>
       </c>
       <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
         <v>162</v>
       </c>
-      <c r="E25" t="s">
-        <v>160</v>
-      </c>
-      <c r="F25" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26">
-        <v>24</v>
+      <c r="B26" t="s">
+        <v>169</v>
       </c>
       <c r="C26" t="s">
         <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E26" t="s">
         <v>167</v>
@@ -2842,31 +2980,50 @@
       <c r="F26" t="s">
         <v>168</v>
       </c>
-      <c r="G26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27">
-        <v>25</v>
+      <c r="B27" t="s">
+        <v>172</v>
       </c>
       <c r="C27" t="s">
         <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E27" t="s">
         <v>172</v>
       </c>
       <c r="F27" t="s">
-        <v>173</v>
-      </c>
-      <c r="G27" t="s">
-        <v>175</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="D28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="D29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="D31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="D32" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6th random albums don't dupe
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24860" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="198">
   <si>
     <t>Album Match</t>
   </si>
@@ -603,6 +603,18 @@
   </si>
   <si>
     <t>how to pull a Var into a document.write function</t>
+  </si>
+  <si>
+    <t>function albumClick</t>
+  </si>
+  <si>
+    <t>the player function that selects the album</t>
+  </si>
+  <si>
+    <t>function gameFinish</t>
+  </si>
+  <si>
+    <t>function nextRound</t>
   </si>
 </sst>
 </file>
@@ -816,8 +828,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -988,7 +1010,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1048,6 +1070,11 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1107,6 +1134,11 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2378,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B20"/>
+  <dimension ref="B2:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2411,36 +2443,56 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="1" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" s="1" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
7th rewrote as objects
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="200">
   <si>
     <t>Album Match</t>
   </si>
@@ -575,12 +575,6 @@
     <t>function songPlay</t>
   </si>
   <si>
-    <t>function logPoint</t>
-  </si>
-  <si>
-    <t>function displayCorrectWrong</t>
-  </si>
-  <si>
     <t>will log a point if the correct album is clicked</t>
   </si>
   <si>
@@ -590,12 +584,6 @@
     <t>function displayScores</t>
   </si>
   <si>
-    <t>needs to play one of the 4 songs by populating the audio tag in the html page</t>
-  </si>
-  <si>
-    <t>needs to randomly choose the song from the album array</t>
-  </si>
-  <si>
     <t>make this a function of the getWinner function</t>
   </si>
   <si>
@@ -615,6 +603,24 @@
   </si>
   <si>
     <t>function nextRound</t>
+  </si>
+  <si>
+    <t>function logPoint  displayCorrectWrong</t>
+  </si>
+  <si>
+    <t>function nextPlayer</t>
+  </si>
+  <si>
+    <t>play a random song from one of 4 albums by populating the audio tag in the html</t>
+  </si>
+  <si>
+    <t>these are separate arrays now- albums and songs</t>
+  </si>
+  <si>
+    <t>var roundCount = 1;</t>
+  </si>
+  <si>
+    <t>var playerCount = 1;</t>
   </si>
 </sst>
 </file>
@@ -828,8 +834,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1010,7 +1054,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1075,6 +1119,25 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1139,6 +1202,25 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2410,90 +2492,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B33"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
9th albums and song workinggit add .
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24920" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Status" sheetId="3" r:id="rId2"/>
-    <sheet name="SongList" sheetId="2" r:id="rId3"/>
+    <sheet name="Status" sheetId="3" r:id="rId1"/>
+    <sheet name="SongList" sheetId="2" r:id="rId2"/>
+    <sheet name="Overview" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
   <si>
     <t>Album Match</t>
   </si>
@@ -621,6 +621,30 @@
   </si>
   <si>
     <t>var playerCount = 1;</t>
+  </si>
+  <si>
+    <t>var song1 = {songFile:"xxxx", albumImage:"xxxx"};</t>
+  </si>
+  <si>
+    <t>access it by:</t>
+  </si>
+  <si>
+    <t>objectName.propertyName</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>objectName[propertyName]</t>
+  </si>
+  <si>
+    <t>var song2 = {songFile:"xxxx", albumImage:"xxxx"};</t>
+  </si>
+  <si>
+    <t>BeatIt</t>
+  </si>
+  <si>
+    <t>Bad</t>
   </si>
 </sst>
 </file>
@@ -834,8 +858,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1054,7 +1082,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1138,6 +1166,8 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1221,6 +1251,8 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1550,10 +1582,734 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="D18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="D20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="147.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="D28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="D29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="D31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="D32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I100"/>
   <sheetViews>
     <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:B105"/>
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2488,695 +3244,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="D9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="147.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" t="s">
-        <v>161</v>
-      </c>
-      <c r="D25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>169</v>
-      </c>
-      <c r="C26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" t="s">
-        <v>166</v>
-      </c>
-      <c r="E26" t="s">
-        <v>167</v>
-      </c>
-      <c r="F26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>172</v>
-      </c>
-      <c r="C27" t="s">
-        <v>173</v>
-      </c>
-      <c r="D27" t="s">
-        <v>171</v>
-      </c>
-      <c r="E27" t="s">
-        <v>172</v>
-      </c>
-      <c r="F27" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="D28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="D29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="D30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="D31" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="D32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
12th player works, correct answer doesn't
</commit_message>
<xml_diff>
--- a/Project1.xlsx
+++ b/Project1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25000" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="302">
   <si>
     <t>Album Match</t>
   </si>
@@ -846,6 +846,90 @@
   </si>
   <si>
     <t>1,3,5,7,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    correctWrong.innerHTML = "Correct Answer!";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    currentPlayer.score += 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    playerRound = playerRound + 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    randomAlbumArray();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    newRandomSong();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    correctWrong.innerHTML = "Wrong Answer!";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    playerTurn.innerHTML = "Player 1 Turn";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    playerTurn.innerHTML = "Player 2 Turn";</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>playerTurn.innerHTML = "Player 1 Wins!"</t>
+  </si>
+  <si>
+    <t>playerTurn.innerHTML = "Player 2 Wins!"</t>
+  </si>
+  <si>
+    <t>} else {</t>
+  </si>
+  <si>
+    <t>if ((playerRound % 2 === 0) &amp;&amp; (currentSong === playerSelection) &amp;&amp; (playerRound &lt; 9)) {</t>
+  </si>
+  <si>
+    <t>} else if ((currentSong !== playerSelection) &amp;&amp; (playerRound &lt; 9)) {</t>
+  </si>
+  <si>
+    <t>} else if ((currentSong === playerSelection) &amp;&amp; (playerRound &lt; 9)) {</t>
+  </si>
+  <si>
+    <t>Player 1 Right</t>
+  </si>
+  <si>
+    <t>Player 1 Wrong</t>
+  </si>
+  <si>
+    <t>} else if ((playerRound % 2 === 0) &amp;&amp; (currentSong !== playerSelection) &amp;&amp; (playerRound &lt; 9)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player 2 Right </t>
+  </si>
+  <si>
+    <t>Player 2 Wrong</t>
+  </si>
+  <si>
+    <t>} else if (playerRound =9){</t>
+  </si>
+  <si>
+    <t>Game End- Player 1 Wins</t>
+  </si>
+  <si>
+    <t>Game End- Player 2 Wins</t>
+  </si>
+  <si>
+    <t>need to start by listing Player 1 Turn on load</t>
+  </si>
+  <si>
+    <t>when game finishes list:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game Over </t>
+  </si>
+  <si>
+    <t>Player 1 Wins 5 to 3</t>
+  </si>
+  <si>
+    <t>Player 2 Wins 4 to 2</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1143,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="233">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1345,7 +1471,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="233">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1462,6 +1588,27 @@
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1578,6 +1725,27 @@
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1907,15 +2075,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
+  <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -2036,6 +2205,219 @@
     <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="C35" t="s">
+        <v>289</v>
+      </c>
+      <c r="D35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="D36" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="D37" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="D38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="D39" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4">
+      <c r="D40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4">
+      <c r="D41" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4">
+      <c r="C42" t="s">
+        <v>290</v>
+      </c>
+      <c r="D42" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4">
+      <c r="D43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="D44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4">
+      <c r="D45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4">
+      <c r="D46" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4">
+      <c r="D47" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4">
+      <c r="D48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" t="s">
+        <v>292</v>
+      </c>
+      <c r="D49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="D50" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="D51" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="D52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="D53" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="D54" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="D55" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" t="s">
+        <v>293</v>
+      </c>
+      <c r="D56" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4">
+      <c r="D57" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4">
+      <c r="D58" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4">
+      <c r="D59" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4">
+      <c r="D60" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4">
+      <c r="D61" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4">
+      <c r="D62" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4">
+      <c r="C63" t="s">
+        <v>295</v>
+      </c>
+      <c r="D63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4">
+      <c r="D64" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="D65" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="C66" t="s">
+        <v>296</v>
+      </c>
+      <c r="D66" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="D67" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="D68" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2053,9 +2435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F55"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>